<commit_message>
Changes to raw imu processing
</commit_message>
<xml_diff>
--- a/emg_data.xlsx
+++ b/emg_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\OneDrive\Desktop\Università\Tesi_Master\GitHub\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\giaco\OneDrive\Desktop\Università\Tesi_Master\GitHub\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5719777B-F7FD-4F31-A771-81183D8E9DA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A9DA64-E41F-4420-B97D-A8792D6FAFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="6480" xr2:uid="{9C722CCF-47F2-441F-BFF8-7A3E3BF06167}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12960" xr2:uid="{9C722CCF-47F2-441F-BFF8-7A3E3BF06167}"/>
   </bookViews>
   <sheets>
     <sheet name="Data In" sheetId="2" r:id="rId1"/>
@@ -1015,7 +1015,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BDD43A-8237-4D20-8FF2-D52CEAC3ADFC}">
   <dimension ref="A1:L507"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="82" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1108,16 +1108,16 @@
     </row>
     <row r="5" spans="1:11" s="38" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="22">
-        <v>0.18877730324074074</v>
+        <v>0.17821233796296296</v>
       </c>
       <c r="B5" s="7">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C5" s="7">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D5" s="7">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
@@ -1190,16 +1190,16 @@
     </row>
     <row r="8" spans="1:11" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="34">
-        <v>0.18877730324074074</v>
+        <v>0.17821233796296296</v>
       </c>
       <c r="B8" s="28">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C8" s="28">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D8" s="28">
-        <v>16</v>
+        <v>57</v>
       </c>
       <c r="E8" s="29"/>
       <c r="F8" s="28"/>
@@ -1211,16 +1211,16 @@
     </row>
     <row r="9" spans="1:11" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23">
-        <v>0.18877614583333333</v>
+        <v>0.17821107638888889</v>
       </c>
       <c r="B9" s="20">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C9" s="20">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D9" s="20">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
@@ -1232,16 +1232,16 @@
     </row>
     <row r="10" spans="1:11" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="23">
-        <v>0.18877489583333334</v>
+        <v>0.17820998842592595</v>
       </c>
       <c r="B10" s="20">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C10" s="20">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D10" s="20">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="20"/>
@@ -1253,16 +1253,16 @@
     </row>
     <row r="11" spans="1:11" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="23">
-        <v>0.18877376157407408</v>
+        <v>0.17820872685185185</v>
       </c>
       <c r="B11" s="20">
-        <v>50</v>
+        <v>107</v>
       </c>
       <c r="C11" s="20">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="D11" s="20">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="20"/>
@@ -1274,16 +1274,16 @@
     </row>
     <row r="12" spans="1:11" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
-        <v>0.18877253472222222</v>
+        <v>0.17820763888888888</v>
       </c>
       <c r="B12" s="20">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C12" s="20">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="D12" s="20">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="20"/>
@@ -1295,16 +1295,16 @@
     </row>
     <row r="13" spans="1:11" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="23">
-        <v>0.1887714699074074</v>
+        <v>0.17820637731481481</v>
       </c>
       <c r="B13" s="20">
-        <v>73</v>
+        <v>112</v>
       </c>
       <c r="C13" s="20">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D13" s="20">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="20"/>
@@ -1316,16 +1316,16 @@
     </row>
     <row r="14" spans="1:11" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="23">
-        <v>0.18877026620370371</v>
+        <v>0.17820528935185184</v>
       </c>
       <c r="B14" s="20">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="C14" s="20">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D14" s="20">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
@@ -1337,16 +1337,16 @@
     </row>
     <row r="15" spans="1:11" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="23">
-        <v>0.18876905092592594</v>
+        <v>0.1782042013888889</v>
       </c>
       <c r="B15" s="20">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="C15" s="20">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="D15" s="20">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="20"/>
@@ -1358,16 +1358,16 @@
     </row>
     <row r="16" spans="1:11" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="23">
-        <v>0.18876796296296297</v>
+        <v>0.17820293981481483</v>
       </c>
       <c r="B16" s="20">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="C16" s="20">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="D16" s="20">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="20"/>
@@ -1379,16 +1379,16 @@
     </row>
     <row r="17" spans="1:12" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="23">
-        <v>0.18876679398148147</v>
+        <v>0.17820185185185183</v>
       </c>
       <c r="B17" s="20">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="C17" s="20">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="D17" s="20">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="20"/>
@@ -1400,16 +1400,16 @@
     </row>
     <row r="18" spans="1:12" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
-        <v>0.18876562499999999</v>
+        <v>0.17820059027777779</v>
       </c>
       <c r="B18" s="20">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C18" s="20">
-        <v>87</v>
+        <v>35</v>
       </c>
       <c r="D18" s="20">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
@@ -1421,16 +1421,16 @@
     </row>
     <row r="19" spans="1:12" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="23">
-        <v>0.18876446759259261</v>
+        <v>0.17819950231481482</v>
       </c>
       <c r="B19" s="20">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="C19" s="20">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="D19" s="20">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
@@ -1442,16 +1442,16 @@
     </row>
     <row r="20" spans="1:12" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="23">
-        <v>0.1887633449074074</v>
+        <v>0.17819822916666667</v>
       </c>
       <c r="B20" s="20">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C20" s="20">
-        <v>66</v>
+        <v>24</v>
       </c>
       <c r="D20" s="20">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="E20" s="20"/>
       <c r="F20" s="20"/>
@@ -1463,16 +1463,16 @@
     </row>
     <row r="21" spans="1:12" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="23">
-        <v>0.18876216435185184</v>
+        <v>0.17819707175925928</v>
       </c>
       <c r="B21" s="20">
-        <v>205</v>
+        <v>84</v>
       </c>
       <c r="C21" s="20">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="D21" s="20">
-        <v>122</v>
+        <v>54</v>
       </c>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
@@ -1484,16 +1484,16 @@
     </row>
     <row r="22" spans="1:12" s="25" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="35">
-        <v>0.18876097222222224</v>
+        <v>0.17819590277777778</v>
       </c>
       <c r="B22" s="32">
-        <v>152</v>
+        <v>72</v>
       </c>
       <c r="C22" s="32">
-        <v>86</v>
+        <v>34</v>
       </c>
       <c r="D22" s="32">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="E22" s="32"/>
       <c r="F22" s="32"/>
@@ -1508,16 +1508,16 @@
     </row>
     <row r="23" spans="1:12" s="25" customFormat="1" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A23" s="36">
-        <v>0.18875973379629629</v>
+        <v>0.17819474537037036</v>
       </c>
       <c r="B23" s="24">
-        <v>222</v>
+        <v>54</v>
       </c>
       <c r="C23" s="24">
-        <v>86</v>
+        <v>28</v>
       </c>
       <c r="D23" s="24">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="E23" s="24"/>
       <c r="F23" s="24"/>
@@ -1529,16 +1529,16 @@
     </row>
     <row r="24" spans="1:12" s="25" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="36">
-        <v>0.18875859953703705</v>
+        <v>0.17819358796296295</v>
       </c>
       <c r="B24" s="24">
-        <v>187</v>
+        <v>33</v>
       </c>
       <c r="C24" s="24">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="D24" s="24">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="E24" s="24"/>
       <c r="F24" s="24"/>
@@ -1550,16 +1550,16 @@
     </row>
     <row r="25" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="36">
-        <v>0.18875744212962964</v>
+        <v>0.1781924189814815</v>
       </c>
       <c r="B25" s="24">
-        <v>81</v>
+        <v>25</v>
       </c>
       <c r="C25" s="24">
-        <v>85</v>
+        <v>26</v>
       </c>
       <c r="D25" s="24">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E25" s="24"/>
       <c r="F25" s="24"/>
@@ -1571,16 +1571,16 @@
     </row>
     <row r="26" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="36">
-        <v>0.18875629629629628</v>
+        <v>0.17819127314814814</v>
       </c>
       <c r="B26" s="24">
-        <v>119</v>
+        <v>15</v>
       </c>
       <c r="C26" s="24">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="D26" s="24">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="E26" s="24"/>
       <c r="F26" s="24"/>
@@ -1592,16 +1592,16 @@
     </row>
     <row r="27" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="36">
-        <v>0.1887550925925926</v>
+        <v>0.17819010416666667</v>
       </c>
       <c r="B27" s="24">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="C27" s="24">
-        <v>119</v>
+        <v>27</v>
       </c>
       <c r="D27" s="24">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
@@ -1613,16 +1613,16 @@
     </row>
     <row r="28" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="36">
-        <v>0.18875393518518518</v>
+        <v>0.17818895833333334</v>
       </c>
       <c r="B28" s="24">
-        <v>269</v>
+        <v>15</v>
       </c>
       <c r="C28" s="24">
-        <v>135</v>
+        <v>29</v>
       </c>
       <c r="D28" s="24">
-        <v>200</v>
+        <v>54</v>
       </c>
       <c r="E28" s="24"/>
       <c r="F28" s="24"/>
@@ -1634,16 +1634,16 @@
     </row>
     <row r="29" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="36">
-        <v>0.18875276620370371</v>
+        <v>0.17818778935185184</v>
       </c>
       <c r="B29" s="24">
-        <v>274</v>
+        <v>24</v>
       </c>
       <c r="C29" s="24">
-        <v>285</v>
+        <v>32</v>
       </c>
       <c r="D29" s="24">
-        <v>275</v>
+        <v>55</v>
       </c>
       <c r="E29" s="24"/>
       <c r="F29" s="24"/>
@@ -1655,16 +1655,16 @@
     </row>
     <row r="30" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="36">
-        <v>0.18875159722222223</v>
+        <v>0.17818663194444445</v>
       </c>
       <c r="B30" s="24">
-        <v>340</v>
+        <v>42</v>
       </c>
       <c r="C30" s="24">
-        <v>491</v>
+        <v>30</v>
       </c>
       <c r="D30" s="24">
-        <v>407</v>
+        <v>55</v>
       </c>
       <c r="E30" s="24"/>
       <c r="F30" s="24"/>
@@ -1676,16 +1676,16 @@
     </row>
     <row r="31" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="36">
-        <v>0.18875041666666667</v>
+        <v>0.17818546296296298</v>
       </c>
       <c r="B31" s="24">
-        <v>271</v>
+        <v>59</v>
       </c>
       <c r="C31" s="24">
-        <v>355</v>
+        <v>33</v>
       </c>
       <c r="D31" s="24">
-        <v>323</v>
+        <v>56</v>
       </c>
       <c r="E31" s="24"/>
       <c r="F31" s="24"/>
@@ -1697,16 +1697,16 @@
     </row>
     <row r="32" spans="1:12" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="36">
-        <v>0.18874925925925926</v>
+        <v>0.17818430555555556</v>
       </c>
       <c r="B32" s="24">
-        <v>123</v>
+        <v>45</v>
       </c>
       <c r="C32" s="24">
-        <v>295</v>
+        <v>32</v>
       </c>
       <c r="D32" s="24">
-        <v>209</v>
+        <v>56</v>
       </c>
       <c r="E32" s="24"/>
       <c r="F32" s="24"/>
@@ -1718,16 +1718,16 @@
     </row>
     <row r="33" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="36">
-        <v>0.18874810185185184</v>
+        <v>0.17818313657407406</v>
       </c>
       <c r="B33" s="24">
-        <v>77</v>
+        <v>44</v>
       </c>
       <c r="C33" s="24">
-        <v>180</v>
+        <v>32</v>
       </c>
       <c r="D33" s="24">
-        <v>172</v>
+        <v>58</v>
       </c>
       <c r="E33" s="24"/>
       <c r="F33" s="24"/>
@@ -1739,16 +1739,16 @@
     </row>
     <row r="34" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="36">
-        <v>0.18874694444444445</v>
+        <v>0.17818197916666667</v>
       </c>
       <c r="B34" s="24">
-        <v>156</v>
+        <v>11</v>
       </c>
       <c r="C34" s="24">
-        <v>227</v>
+        <v>36</v>
       </c>
       <c r="D34" s="24">
-        <v>217</v>
+        <v>60</v>
       </c>
       <c r="E34" s="24"/>
       <c r="F34" s="24"/>
@@ -1760,16 +1760,16 @@
     </row>
     <row r="35" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="36">
-        <v>0.18874577546296298</v>
+        <v>0.17818082175925926</v>
       </c>
       <c r="B35" s="24">
-        <v>143</v>
+        <v>11</v>
       </c>
       <c r="C35" s="24">
-        <v>267</v>
+        <v>40</v>
       </c>
       <c r="D35" s="24">
-        <v>246</v>
+        <v>65</v>
       </c>
       <c r="E35" s="24"/>
       <c r="F35" s="24"/>
@@ -1781,16 +1781,16 @@
     </row>
     <row r="36" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="36">
-        <v>0.18874466435185186</v>
+        <v>0.17817966435185184</v>
       </c>
       <c r="B36" s="24">
-        <v>317</v>
+        <v>26</v>
       </c>
       <c r="C36" s="24">
-        <v>293</v>
+        <v>49</v>
       </c>
       <c r="D36" s="24">
-        <v>190</v>
+        <v>71</v>
       </c>
       <c r="E36" s="24"/>
       <c r="F36" s="24"/>
@@ -1802,16 +1802,16 @@
     </row>
     <row r="37" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="36">
-        <v>0.18874329861111111</v>
+        <v>0.17817849537037037</v>
       </c>
       <c r="B37" s="24">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="C37" s="24">
-        <v>346</v>
+        <v>56</v>
       </c>
       <c r="D37" s="24">
-        <v>144</v>
+        <v>73</v>
       </c>
       <c r="E37" s="24"/>
       <c r="F37" s="24"/>
@@ -1823,16 +1823,16 @@
     </row>
     <row r="38" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="36">
-        <v>0.18874230324074073</v>
+        <v>0.17817733796296298</v>
       </c>
       <c r="B38" s="24">
-        <v>93</v>
+        <v>15</v>
       </c>
       <c r="C38" s="24">
-        <v>475</v>
+        <v>45</v>
       </c>
       <c r="D38" s="24">
-        <v>103</v>
+        <v>69</v>
       </c>
       <c r="E38" s="24"/>
       <c r="F38" s="24"/>
@@ -1844,16 +1844,16 @@
     </row>
     <row r="39" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="36">
-        <v>0.1887411226851852</v>
+        <v>0.17817618055555556</v>
       </c>
       <c r="B39" s="24">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="C39" s="24">
-        <v>630</v>
+        <v>48</v>
       </c>
       <c r="D39" s="24">
-        <v>118</v>
+        <v>72</v>
       </c>
       <c r="E39" s="24"/>
       <c r="F39" s="24"/>
@@ -1865,16 +1865,16 @@
     </row>
     <row r="40" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="36">
-        <v>0.18873995370370369</v>
+        <v>0.17817502314814815</v>
       </c>
       <c r="B40" s="24">
-        <v>102</v>
+        <v>17</v>
       </c>
       <c r="C40" s="24">
-        <v>527</v>
+        <v>60</v>
       </c>
       <c r="D40" s="24">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="E40" s="24"/>
       <c r="F40" s="24"/>
@@ -1886,16 +1886,16 @@
     </row>
     <row r="41" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="36">
-        <v>0.18873877314814816</v>
+        <v>0.17817386574074073</v>
       </c>
       <c r="B41" s="24">
-        <v>123</v>
+        <v>22</v>
       </c>
       <c r="C41" s="24">
-        <v>394</v>
+        <v>52</v>
       </c>
       <c r="D41" s="24">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E41" s="24"/>
       <c r="F41" s="24"/>
@@ -1907,16 +1907,16 @@
     </row>
     <row r="42" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="36">
-        <v>0.18873760416666666</v>
+        <v>0.17817269675925926</v>
       </c>
       <c r="B42" s="24">
-        <v>86</v>
+        <v>25</v>
       </c>
       <c r="C42" s="24">
-        <v>369</v>
+        <v>62</v>
       </c>
       <c r="D42" s="24">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="E42" s="24"/>
       <c r="F42" s="24"/>
@@ -1928,16 +1928,16 @@
     </row>
     <row r="43" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="36">
-        <v>0.18873642361111109</v>
+        <v>0.17817153935185187</v>
       </c>
       <c r="B43" s="24">
-        <v>168</v>
+        <v>26</v>
       </c>
       <c r="C43" s="24">
-        <v>332</v>
+        <v>63</v>
       </c>
       <c r="D43" s="24">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="E43" s="24"/>
       <c r="F43" s="24"/>
@@ -1949,16 +1949,16 @@
     </row>
     <row r="44" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="36">
-        <v>0.18873527777777777</v>
+        <v>0.17817037037037037</v>
       </c>
       <c r="B44" s="24">
-        <v>148</v>
+        <v>35</v>
       </c>
       <c r="C44" s="24">
-        <v>292</v>
+        <v>68</v>
       </c>
       <c r="D44" s="24">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="E44" s="24"/>
       <c r="F44" s="24"/>
@@ -1970,16 +1970,16 @@
     </row>
     <row r="45" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="36">
-        <v>0.18873494212962963</v>
+        <v>0.17816921296296295</v>
       </c>
       <c r="B45" s="24">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="C45" s="24">
-        <v>243</v>
+        <v>69</v>
       </c>
       <c r="D45" s="24">
-        <v>41</v>
+        <v>91</v>
       </c>
       <c r="E45" s="24"/>
       <c r="F45" s="24"/>
@@ -1991,16 +1991,16 @@
     </row>
     <row r="46" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="36">
-        <v>0.18873296296296296</v>
+        <v>0.17816805555555554</v>
       </c>
       <c r="B46" s="24">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="C46" s="24">
-        <v>117</v>
+        <v>69</v>
       </c>
       <c r="D46" s="24">
-        <v>26</v>
+        <v>97</v>
       </c>
       <c r="E46" s="24"/>
       <c r="F46" s="24"/>
@@ -2012,16 +2012,16 @@
     </row>
     <row r="47" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="36">
-        <v>0.18873167824074075</v>
+        <v>0.17816671296296296</v>
       </c>
       <c r="B47" s="24">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="C47" s="24">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D47" s="24">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="E47" s="24"/>
       <c r="F47" s="24"/>
@@ -2033,16 +2033,16 @@
     </row>
     <row r="48" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="36">
-        <v>0.18873054398148148</v>
+        <v>0.17816572916666668</v>
       </c>
       <c r="B48" s="24">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="C48" s="24">
-        <v>71</v>
+        <v>103</v>
       </c>
       <c r="D48" s="24">
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="E48" s="24"/>
       <c r="F48" s="24"/>
@@ -2054,16 +2054,16 @@
     </row>
     <row r="49" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="36">
-        <v>0.18872936342592594</v>
+        <v>0.17816438657407407</v>
       </c>
       <c r="B49" s="24">
-        <v>0</v>
+        <v>105</v>
       </c>
       <c r="C49" s="24">
-        <v>68</v>
+        <v>145</v>
       </c>
       <c r="D49" s="24">
-        <v>0</v>
+        <v>231</v>
       </c>
       <c r="E49" s="24"/>
       <c r="F49" s="24"/>
@@ -2075,16 +2075,16 @@
     </row>
     <row r="50" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="36">
-        <v>0.18872828703703703</v>
+        <v>0.17816322916666666</v>
       </c>
       <c r="B50" s="24">
-        <v>9</v>
+        <v>155</v>
       </c>
       <c r="C50" s="24">
-        <v>52</v>
+        <v>301</v>
       </c>
       <c r="D50" s="24">
-        <v>0</v>
+        <v>385</v>
       </c>
       <c r="E50" s="24"/>
       <c r="F50" s="24"/>
@@ -2096,16 +2096,16 @@
     </row>
     <row r="51" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="36">
-        <v>0.18872702546296297</v>
+        <v>0.17816207175925924</v>
       </c>
       <c r="B51" s="24">
-        <v>123</v>
+        <v>280</v>
       </c>
       <c r="C51" s="24">
-        <v>45</v>
+        <v>509</v>
       </c>
       <c r="D51" s="24">
-        <v>152</v>
+        <v>546</v>
       </c>
       <c r="E51" s="24"/>
       <c r="F51" s="24"/>
@@ -2117,16 +2117,16 @@
     </row>
     <row r="52" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="36">
-        <v>0.18872592592592594</v>
+        <v>0.17816089120370371</v>
       </c>
       <c r="B52" s="24">
-        <v>26</v>
+        <v>449</v>
       </c>
       <c r="C52" s="24">
-        <v>42</v>
+        <v>636</v>
       </c>
       <c r="D52" s="24">
-        <v>16</v>
+        <v>633</v>
       </c>
       <c r="E52" s="24"/>
       <c r="F52" s="24"/>
@@ -2138,16 +2138,16 @@
     </row>
     <row r="53" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="36">
-        <v>0.18872473379629628</v>
+        <v>0.17815973379629629</v>
       </c>
       <c r="B53" s="24">
-        <v>103</v>
+        <v>484</v>
       </c>
       <c r="C53" s="24">
-        <v>37</v>
+        <v>715</v>
       </c>
       <c r="D53" s="24">
-        <v>17</v>
+        <v>654</v>
       </c>
       <c r="E53" s="24"/>
       <c r="F53" s="24"/>
@@ -2159,16 +2159,16 @@
     </row>
     <row r="54" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="36">
-        <v>0.18872363425925925</v>
+        <v>0.17815857638888888</v>
       </c>
       <c r="B54" s="24">
-        <v>51</v>
+        <v>458</v>
       </c>
       <c r="C54" s="24">
-        <v>39</v>
+        <v>609</v>
       </c>
       <c r="D54" s="24">
-        <v>14</v>
+        <v>567</v>
       </c>
       <c r="E54" s="24"/>
       <c r="F54" s="24"/>
@@ -2180,16 +2180,16 @@
     </row>
     <row r="55" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="36">
-        <v>0.18872246527777778</v>
+        <v>0.17815741898148146</v>
       </c>
       <c r="B55" s="24">
-        <v>32</v>
+        <v>358</v>
       </c>
       <c r="C55" s="24">
-        <v>44</v>
+        <v>560</v>
       </c>
       <c r="D55" s="24">
-        <v>14</v>
+        <v>511</v>
       </c>
       <c r="E55" s="24"/>
       <c r="F55" s="24"/>
@@ -2201,16 +2201,16 @@
     </row>
     <row r="56" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="36">
-        <v>0.18872119212962962</v>
+        <v>0.17815625000000002</v>
       </c>
       <c r="B56" s="24">
-        <v>58</v>
+        <v>497</v>
       </c>
       <c r="C56" s="24">
-        <v>43</v>
+        <v>429</v>
       </c>
       <c r="D56" s="24">
-        <v>14</v>
+        <v>438</v>
       </c>
       <c r="E56" s="24"/>
       <c r="F56" s="24"/>
@@ -2222,16 +2222,16 @@
     </row>
     <row r="57" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="36">
-        <v>0.18871994212962964</v>
+        <v>0.1781550925925926</v>
       </c>
       <c r="B57" s="24">
-        <v>70</v>
+        <v>395</v>
       </c>
       <c r="C57" s="24">
-        <v>44</v>
+        <v>445</v>
       </c>
       <c r="D57" s="24">
-        <v>12</v>
+        <v>466</v>
       </c>
       <c r="E57" s="24"/>
       <c r="F57" s="24"/>
@@ -2243,16 +2243,16 @@
     </row>
     <row r="58" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="36">
-        <v>0.18871886574074073</v>
+        <v>0.1781539236111111</v>
       </c>
       <c r="B58" s="24">
-        <v>75</v>
+        <v>350</v>
       </c>
       <c r="C58" s="24">
-        <v>44</v>
+        <v>500</v>
       </c>
       <c r="D58" s="24">
-        <v>10</v>
+        <v>517</v>
       </c>
       <c r="E58" s="24"/>
       <c r="F58" s="24"/>
@@ -2264,16 +2264,16 @@
     </row>
     <row r="59" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="36">
-        <v>0.18871777777777779</v>
+        <v>0.17815276620370371</v>
       </c>
       <c r="B59" s="24">
-        <v>67</v>
+        <v>339</v>
       </c>
       <c r="C59" s="24">
-        <v>43</v>
+        <v>577</v>
       </c>
       <c r="D59" s="24">
-        <v>10</v>
+        <v>567</v>
       </c>
       <c r="E59" s="24"/>
       <c r="F59" s="24"/>
@@ -2285,16 +2285,16 @@
     </row>
     <row r="60" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="36">
-        <v>0.18871655092592593</v>
+        <v>0.17815159722222224</v>
       </c>
       <c r="B60" s="24">
-        <v>60</v>
+        <v>297</v>
       </c>
       <c r="C60" s="24">
-        <v>44</v>
+        <v>596</v>
       </c>
       <c r="D60" s="24">
-        <v>10</v>
+        <v>567</v>
       </c>
       <c r="E60" s="24"/>
       <c r="F60" s="24"/>
@@ -2306,16 +2306,16 @@
     </row>
     <row r="61" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="36">
-        <v>0.18871546296296296</v>
+        <v>0.17815043981481482</v>
       </c>
       <c r="B61" s="24">
-        <v>55</v>
+        <v>210</v>
       </c>
       <c r="C61" s="24">
-        <v>43</v>
+        <v>503</v>
       </c>
       <c r="D61" s="24">
-        <v>11</v>
+        <v>532</v>
       </c>
       <c r="E61" s="24"/>
       <c r="F61" s="24"/>
@@ -2327,16 +2327,16 @@
     </row>
     <row r="62" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="36">
-        <v>0.1887142361111111</v>
+        <v>0.17814928240740741</v>
       </c>
       <c r="B62" s="24">
-        <v>52</v>
+        <v>213</v>
       </c>
       <c r="C62" s="24">
-        <v>42</v>
+        <v>651</v>
       </c>
       <c r="D62" s="24">
-        <v>14</v>
+        <v>603</v>
       </c>
       <c r="E62" s="24"/>
       <c r="F62" s="24"/>
@@ -2348,16 +2348,16 @@
     </row>
     <row r="63" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="36">
-        <v>0.18871307870370368</v>
+        <v>0.17814811342592593</v>
       </c>
       <c r="B63" s="24">
-        <v>50</v>
+        <v>206</v>
       </c>
       <c r="C63" s="24">
-        <v>43</v>
+        <v>532</v>
       </c>
       <c r="D63" s="24">
-        <v>11</v>
+        <v>535</v>
       </c>
       <c r="E63" s="24"/>
       <c r="F63" s="24"/>
@@ -2369,16 +2369,16 @@
     </row>
     <row r="64" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="36">
-        <v>0.18871190972222224</v>
+        <v>0.17814695601851852</v>
       </c>
       <c r="B64" s="24">
-        <v>49</v>
+        <v>196</v>
       </c>
       <c r="C64" s="24">
-        <v>43</v>
+        <v>616</v>
       </c>
       <c r="D64" s="24">
-        <v>10</v>
+        <v>562</v>
       </c>
       <c r="E64" s="24"/>
       <c r="F64" s="24"/>
@@ -2390,16 +2390,16 @@
     </row>
     <row r="65" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="36">
-        <v>0.18871077546296297</v>
+        <v>0.17814579861111113</v>
       </c>
       <c r="B65" s="24">
-        <v>50</v>
+        <v>152</v>
       </c>
       <c r="C65" s="24">
-        <v>44</v>
+        <v>515</v>
       </c>
       <c r="D65" s="24">
-        <v>9</v>
+        <v>487</v>
       </c>
       <c r="E65" s="24"/>
       <c r="F65" s="24"/>
@@ -2411,16 +2411,16 @@
     </row>
     <row r="66" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="36">
-        <v>0.1887096064814815</v>
+        <v>0.17814464120370371</v>
       </c>
       <c r="B66" s="24">
-        <v>51</v>
+        <v>146</v>
       </c>
       <c r="C66" s="24">
-        <v>42</v>
+        <v>509</v>
       </c>
       <c r="D66" s="24">
-        <v>8</v>
+        <v>455</v>
       </c>
       <c r="E66" s="24"/>
       <c r="F66" s="24"/>
@@ -2432,16 +2432,16 @@
     </row>
     <row r="67" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="36">
-        <v>0.18870835648148149</v>
+        <v>0.1781434837962963</v>
       </c>
       <c r="B67" s="24">
-        <v>48</v>
+        <v>172</v>
       </c>
       <c r="C67" s="24">
-        <v>43</v>
+        <v>419</v>
       </c>
       <c r="D67" s="24">
-        <v>8</v>
+        <v>371</v>
       </c>
       <c r="E67" s="24"/>
       <c r="F67" s="24"/>
@@ -2453,16 +2453,16 @@
     </row>
     <row r="68" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="36">
-        <v>0.18870710648148148</v>
+        <v>0.1781423148148148</v>
       </c>
       <c r="B68" s="24">
-        <v>43</v>
+        <v>209</v>
       </c>
       <c r="C68" s="24">
-        <v>44</v>
+        <v>308</v>
       </c>
       <c r="D68" s="24">
-        <v>9</v>
+        <v>292</v>
       </c>
       <c r="E68" s="24"/>
       <c r="F68" s="24"/>
@@ -2474,16 +2474,16 @@
     </row>
     <row r="69" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="36">
-        <v>0.18870612268518519</v>
+        <v>0.17814114583333335</v>
       </c>
       <c r="B69" s="24">
-        <v>38</v>
+        <v>276</v>
       </c>
       <c r="C69" s="24">
-        <v>43</v>
+        <v>288</v>
       </c>
       <c r="D69" s="24">
-        <v>8</v>
+        <v>267</v>
       </c>
       <c r="E69" s="24"/>
       <c r="F69" s="24"/>
@@ -2495,16 +2495,16 @@
     </row>
     <row r="70" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="36">
-        <v>0.18870478009259259</v>
+        <v>0.17813998842592593</v>
       </c>
       <c r="B70" s="24">
-        <v>34</v>
+        <v>362</v>
       </c>
       <c r="C70" s="24">
-        <v>44</v>
+        <v>232</v>
       </c>
       <c r="D70" s="24">
-        <v>8</v>
+        <v>225</v>
       </c>
       <c r="E70" s="24"/>
       <c r="F70" s="24"/>
@@ -2516,16 +2516,16 @@
     </row>
     <row r="71" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="36">
-        <v>0.18870380787037036</v>
+        <v>0.17813883101851852</v>
       </c>
       <c r="B71" s="24">
-        <v>32</v>
+        <v>388</v>
       </c>
       <c r="C71" s="24">
-        <v>43</v>
+        <v>209</v>
       </c>
       <c r="D71" s="24">
-        <v>8</v>
+        <v>210</v>
       </c>
       <c r="E71" s="24"/>
       <c r="F71" s="24"/>
@@ -2537,16 +2537,16 @@
     </row>
     <row r="72" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="36">
-        <v>0.18870258101851853</v>
+        <v>0.17813766203703701</v>
       </c>
       <c r="B72" s="24">
-        <v>29</v>
+        <v>547</v>
       </c>
       <c r="C72" s="24">
-        <v>44</v>
+        <v>200</v>
       </c>
       <c r="D72" s="24">
-        <v>8</v>
+        <v>206</v>
       </c>
       <c r="E72" s="24"/>
       <c r="F72" s="24"/>
@@ -2558,16 +2558,16 @@
     </row>
     <row r="73" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="36">
-        <v>0.18870130787037037</v>
+        <v>0.17813650462962963</v>
       </c>
       <c r="B73" s="24">
-        <v>19</v>
+        <v>656</v>
       </c>
       <c r="C73" s="24">
-        <v>43</v>
+        <v>205</v>
       </c>
       <c r="D73" s="24">
-        <v>9</v>
+        <v>212</v>
       </c>
       <c r="E73" s="24"/>
       <c r="F73" s="24"/>
@@ -2579,16 +2579,16 @@
     </row>
     <row r="74" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="36">
-        <v>0.18870015046296296</v>
+        <v>0.17813534722222221</v>
       </c>
       <c r="B74" s="24">
-        <v>9</v>
+        <v>709</v>
       </c>
       <c r="C74" s="24">
-        <v>43</v>
+        <v>210</v>
       </c>
       <c r="D74" s="24">
-        <v>10</v>
+        <v>222</v>
       </c>
       <c r="E74" s="24"/>
       <c r="F74" s="24"/>
@@ -2600,16 +2600,16 @@
     </row>
     <row r="75" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="36">
-        <v>0.18869899305555557</v>
+        <v>0.17813400462962964</v>
       </c>
       <c r="B75" s="24">
-        <v>18</v>
+        <v>718</v>
       </c>
       <c r="C75" s="24">
-        <v>44</v>
+        <v>243</v>
       </c>
       <c r="D75" s="24">
-        <v>9</v>
+        <v>242</v>
       </c>
       <c r="E75" s="24"/>
       <c r="F75" s="24"/>
@@ -2621,16 +2621,16 @@
     </row>
     <row r="76" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="36">
-        <v>0.18869783564814815</v>
+        <v>0.17813284722222222</v>
       </c>
       <c r="B76" s="24">
-        <v>34</v>
+        <v>774</v>
       </c>
       <c r="C76" s="24">
-        <v>44</v>
+        <v>257</v>
       </c>
       <c r="D76" s="24">
-        <v>8</v>
+        <v>243</v>
       </c>
       <c r="E76" s="24"/>
       <c r="F76" s="24"/>
@@ -2642,16 +2642,16 @@
     </row>
     <row r="77" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="36">
-        <v>0.18869675925925924</v>
+        <v>0.17813168981481481</v>
       </c>
       <c r="B77" s="24">
-        <v>43</v>
+        <v>785</v>
       </c>
       <c r="C77" s="24">
-        <v>44</v>
+        <v>223</v>
       </c>
       <c r="D77" s="24">
-        <v>8</v>
+        <v>214</v>
       </c>
       <c r="E77" s="24"/>
       <c r="F77" s="24"/>
@@ -2663,16 +2663,16 @@
     </row>
     <row r="78" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="36">
-        <v>0.18869552083333332</v>
+        <v>0.17813052083333333</v>
       </c>
       <c r="B78" s="24">
-        <v>46</v>
+        <v>790</v>
       </c>
       <c r="C78" s="24">
-        <v>43</v>
+        <v>195</v>
       </c>
       <c r="D78" s="24">
-        <v>8</v>
+        <v>194</v>
       </c>
       <c r="E78" s="24"/>
       <c r="F78" s="24"/>
@@ -2684,16 +2684,16 @@
     </row>
     <row r="79" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="36">
-        <v>0.18869436342592591</v>
+        <v>0.17812936342592592</v>
       </c>
       <c r="B79" s="24">
-        <v>46</v>
+        <v>818</v>
       </c>
       <c r="C79" s="24">
-        <v>43</v>
+        <v>165</v>
       </c>
       <c r="D79" s="24">
-        <v>9</v>
+        <v>183</v>
       </c>
       <c r="E79" s="24"/>
       <c r="F79" s="24"/>
@@ -2705,16 +2705,16 @@
     </row>
     <row r="80" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="36">
-        <v>0.1886933101851852</v>
+        <v>0.17812819444444444</v>
       </c>
       <c r="B80" s="24">
-        <v>43</v>
+        <v>700</v>
       </c>
       <c r="C80" s="24">
-        <v>43</v>
+        <v>200</v>
       </c>
       <c r="D80" s="24">
-        <v>8</v>
+        <v>208</v>
       </c>
       <c r="E80" s="24"/>
       <c r="F80" s="24"/>
@@ -2726,16 +2726,16 @@
     </row>
     <row r="81" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="36">
-        <v>0.18869203703703705</v>
+        <v>0.17812703703703703</v>
       </c>
       <c r="B81" s="24">
-        <v>40</v>
+        <v>604</v>
       </c>
       <c r="C81" s="24">
-        <v>44</v>
+        <v>209</v>
       </c>
       <c r="D81" s="24">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="E81" s="24"/>
       <c r="F81" s="24"/>
@@ -2747,16 +2747,16 @@
     </row>
     <row r="82" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="36">
-        <v>0.18869087962962963</v>
+        <v>0.17812587962962961</v>
       </c>
       <c r="B82" s="24">
-        <v>41</v>
+        <v>386</v>
       </c>
       <c r="C82" s="24">
-        <v>43</v>
+        <v>211</v>
       </c>
       <c r="D82" s="24">
-        <v>7</v>
+        <v>232</v>
       </c>
       <c r="E82" s="24"/>
       <c r="F82" s="24"/>
@@ -2768,16 +2768,16 @@
     </row>
     <row r="83" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="36">
-        <v>0.18868972222222222</v>
+        <v>0.17812472222222223</v>
       </c>
       <c r="B83" s="24">
-        <v>46</v>
+        <v>305</v>
       </c>
       <c r="C83" s="24">
-        <v>43</v>
+        <v>260</v>
       </c>
       <c r="D83" s="24">
-        <v>8</v>
+        <v>270</v>
       </c>
       <c r="E83" s="24"/>
       <c r="F83" s="24"/>
@@ -2789,16 +2789,16 @@
     </row>
     <row r="84" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="36">
-        <v>0.1886885648148148</v>
+        <v>0.17812356481481481</v>
       </c>
       <c r="B84" s="24">
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="C84" s="24">
-        <v>43</v>
+        <v>302</v>
       </c>
       <c r="D84" s="24">
-        <v>9</v>
+        <v>287</v>
       </c>
       <c r="E84" s="24"/>
       <c r="F84" s="24"/>
@@ -2810,16 +2810,16 @@
     </row>
     <row r="85" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="36">
-        <v>0.18868736111111112</v>
+        <v>0.17812239583333334</v>
       </c>
       <c r="B85" s="24">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="C85" s="24">
-        <v>44</v>
+        <v>269</v>
       </c>
       <c r="D85" s="24">
-        <v>10</v>
+        <v>260</v>
       </c>
       <c r="E85" s="24"/>
       <c r="F85" s="24"/>
@@ -2831,16 +2831,16 @@
     </row>
     <row r="86" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="36">
-        <v>0.18868630787037036</v>
+        <v>0.17812123842592592</v>
       </c>
       <c r="B86" s="24">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C86" s="24">
-        <v>44</v>
+        <v>269</v>
       </c>
       <c r="D86" s="24">
-        <v>9</v>
+        <v>245</v>
       </c>
       <c r="E86" s="24"/>
       <c r="F86" s="24"/>
@@ -2852,16 +2852,16 @@
     </row>
     <row r="87" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="36">
-        <v>0.18868501157407408</v>
+        <v>0.17812008101851853</v>
       </c>
       <c r="B87" s="24">
-        <v>45</v>
+        <v>0</v>
       </c>
       <c r="C87" s="24">
-        <v>44</v>
+        <v>215</v>
       </c>
       <c r="D87" s="24">
-        <v>7</v>
+        <v>199</v>
       </c>
       <c r="E87" s="24"/>
       <c r="F87" s="24"/>
@@ -2873,16 +2873,16 @@
     </row>
     <row r="88" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="36">
-        <v>0.18868392361111111</v>
+        <v>0.17811891203703703</v>
       </c>
       <c r="B88" s="24">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="C88" s="24">
-        <v>43</v>
+        <v>154</v>
       </c>
       <c r="D88" s="24">
-        <v>8</v>
+        <v>159</v>
       </c>
       <c r="E88" s="24"/>
       <c r="F88" s="24"/>
@@ -2894,16 +2894,16 @@
     </row>
     <row r="89" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="36">
-        <v>0.18868282407407408</v>
+        <v>0.17811775462962962</v>
       </c>
       <c r="B89" s="24">
-        <v>46</v>
+        <v>185</v>
       </c>
       <c r="C89" s="24">
-        <v>43</v>
+        <v>164</v>
       </c>
       <c r="D89" s="24">
-        <v>9</v>
+        <v>158</v>
       </c>
       <c r="E89" s="24"/>
       <c r="F89" s="24"/>
@@ -2915,16 +2915,16 @@
     </row>
     <row r="90" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="36">
-        <v>0.18868156249999998</v>
+        <v>0.17811659722222223</v>
       </c>
       <c r="B90" s="24">
-        <v>45</v>
+        <v>187</v>
       </c>
       <c r="C90" s="24">
-        <v>40</v>
+        <v>137</v>
       </c>
       <c r="D90" s="24">
-        <v>8</v>
+        <v>132</v>
       </c>
       <c r="E90" s="24"/>
       <c r="F90" s="24"/>
@@ -2936,16 +2936,16 @@
     </row>
     <row r="91" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="36">
-        <v>0.18868059027777778</v>
+        <v>0.17811543981481481</v>
       </c>
       <c r="B91" s="24">
-        <v>45</v>
+        <v>86</v>
       </c>
       <c r="C91" s="24">
-        <v>35</v>
+        <v>93</v>
       </c>
       <c r="D91" s="24">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="E91" s="24"/>
       <c r="F91" s="24"/>
@@ -2957,16 +2957,16 @@
     </row>
     <row r="92" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="36">
-        <v>0.18867929398148148</v>
+        <v>0.17811428240740743</v>
       </c>
       <c r="B92" s="24">
-        <v>44</v>
+        <v>148</v>
       </c>
       <c r="C92" s="24">
-        <v>33</v>
+        <v>66</v>
       </c>
       <c r="D92" s="24">
-        <v>5</v>
+        <v>85</v>
       </c>
       <c r="E92" s="24"/>
       <c r="F92" s="24"/>
@@ -2978,16 +2978,16 @@
     </row>
     <row r="93" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="36">
-        <v>0.18867810185185185</v>
+        <v>0.17811311342592592</v>
       </c>
       <c r="B93" s="24">
-        <v>44</v>
+        <v>297</v>
       </c>
       <c r="C93" s="24">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="D93" s="24">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="E93" s="24"/>
       <c r="F93" s="24"/>
@@ -2999,16 +2999,16 @@
     </row>
     <row r="94" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="36">
-        <v>0.1886770023148148</v>
+        <v>0.17811195601851851</v>
       </c>
       <c r="B94" s="24">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="C94" s="24">
-        <v>32</v>
+        <v>79</v>
       </c>
       <c r="D94" s="24">
-        <v>6</v>
+        <v>85</v>
       </c>
       <c r="E94" s="24"/>
       <c r="F94" s="24"/>
@@ -3020,16 +3020,16 @@
     </row>
     <row r="95" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="36">
-        <v>0.18867562500000001</v>
+        <v>0.17811079861111109</v>
       </c>
       <c r="B95" s="24">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="C95" s="24">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D95" s="24">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="E95" s="24"/>
       <c r="F95" s="24"/>
@@ -3041,16 +3041,16 @@
     </row>
     <row r="96" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="36">
-        <v>0.18867451388888887</v>
+        <v>0.17810957175925926</v>
       </c>
       <c r="B96" s="24">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="C96" s="24">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D96" s="24">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="E96" s="24"/>
       <c r="F96" s="24"/>
@@ -3062,16 +3062,16 @@
     </row>
     <row r="97" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="36">
-        <v>0.18867339120370369</v>
+        <v>0.17810829861111113</v>
       </c>
       <c r="B97" s="24">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C97" s="24">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D97" s="24">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="E97" s="24"/>
       <c r="F97" s="24"/>
@@ -3083,16 +3083,16 @@
     </row>
     <row r="98" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="36">
-        <v>0.1886722800925926</v>
+        <v>0.17810721064814813</v>
       </c>
       <c r="B98" s="24">
-        <v>44</v>
+        <v>87</v>
       </c>
       <c r="C98" s="24">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="D98" s="24">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="E98" s="24"/>
       <c r="F98" s="24"/>
@@ -3104,16 +3104,16 @@
     </row>
     <row r="99" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="36">
-        <v>0.18867097222222223</v>
+        <v>0.17810613425925928</v>
       </c>
       <c r="B99" s="24">
+        <v>76</v>
+      </c>
+      <c r="C99" s="24">
         <v>44</v>
       </c>
-      <c r="C99" s="24">
-        <v>32</v>
-      </c>
       <c r="D99" s="24">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="E99" s="24"/>
       <c r="F99" s="24"/>
@@ -3125,16 +3125,16 @@
     </row>
     <row r="100" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="36">
-        <v>0.18866988425925926</v>
+        <v>0.17810486111111112</v>
       </c>
       <c r="B100" s="24">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="C100" s="24">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="D100" s="24">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="E100" s="24"/>
       <c r="F100" s="24"/>
@@ -3146,16 +3146,16 @@
     </row>
     <row r="101" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="36">
-        <v>0.18866880787037038</v>
+        <v>0.17810378472222221</v>
       </c>
       <c r="B101" s="24">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="C101" s="24">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D101" s="24">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="E101" s="24"/>
       <c r="F101" s="24"/>
@@ -3167,16 +3167,16 @@
     </row>
     <row r="102" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="36">
-        <v>0.18866765046296297</v>
+        <v>0.17810251157407408</v>
       </c>
       <c r="B102" s="24">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="C102" s="24">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="D102" s="24">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="E102" s="24"/>
       <c r="F102" s="24"/>
@@ -3188,16 +3188,16 @@
     </row>
     <row r="103" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="36">
-        <v>0.18866644675925928</v>
+        <v>0.17810142361111111</v>
       </c>
       <c r="B103" s="24">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C103" s="24">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="D103" s="24">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="E103" s="24"/>
       <c r="F103" s="24"/>
@@ -3209,16 +3209,16 @@
     </row>
     <row r="104" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="36">
-        <v>0.18866527777777778</v>
+        <v>0.17810016203703702</v>
       </c>
       <c r="B104" s="24">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C104" s="24">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="D104" s="24">
-        <v>6</v>
+        <v>71</v>
       </c>
       <c r="E104" s="24"/>
       <c r="F104" s="24"/>
@@ -3230,16 +3230,16 @@
     </row>
     <row r="105" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="36">
-        <v>0.18866413194444445</v>
+        <v>0.17809907407407408</v>
       </c>
       <c r="B105" s="24">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="C105" s="24">
-        <v>32</v>
+        <v>51</v>
       </c>
       <c r="D105" s="24">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="E105" s="24"/>
       <c r="F105" s="24"/>
@@ -3251,16 +3251,16 @@
     </row>
     <row r="106" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="36">
-        <v>0.18866287037037036</v>
+        <v>0.17809781250000001</v>
       </c>
       <c r="B106" s="24">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C106" s="24">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="D106" s="24">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="E106" s="24"/>
       <c r="F106" s="24"/>
@@ -3272,16 +3272,16 @@
     </row>
     <row r="107" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="36">
-        <v>0.18866194444444445</v>
+        <v>0.17809672453703704</v>
       </c>
       <c r="B107" s="24">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="C107" s="24">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D107" s="24">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="E107" s="24"/>
       <c r="F107" s="24"/>
@@ -3293,16 +3293,16 @@
     </row>
     <row r="108" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="36">
-        <v>0.18866059027777776</v>
+        <v>0.17809563657407407</v>
       </c>
       <c r="B108" s="24">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C108" s="24">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="D108" s="24">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="E108" s="24"/>
       <c r="F108" s="24"/>
@@ -3314,16 +3314,16 @@
     </row>
     <row r="109" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="36">
-        <v>0.18865944444444444</v>
+        <v>0.178094375</v>
       </c>
       <c r="B109" s="24">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C109" s="24">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="D109" s="24">
-        <v>6</v>
+        <v>69</v>
       </c>
       <c r="E109" s="24"/>
       <c r="F109" s="24"/>
@@ -3335,16 +3335,16 @@
     </row>
     <row r="110" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="36">
-        <v>0.18865818287037037</v>
+        <v>0.17809328703703703</v>
       </c>
       <c r="B110" s="24">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C110" s="24">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="D110" s="24">
-        <v>6</v>
+        <v>68</v>
       </c>
       <c r="E110" s="24"/>
       <c r="F110" s="24"/>
@@ -3356,16 +3356,16 @@
     </row>
     <row r="111" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="36">
-        <v>0.1886570949074074</v>
+        <v>0.17809202546296296</v>
       </c>
       <c r="B111" s="24">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="C111" s="24">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D111" s="24">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="E111" s="24"/>
       <c r="F111" s="24"/>
@@ -3377,16 +3377,16 @@
     </row>
     <row r="112" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="36">
-        <v>0.18865579861111112</v>
+        <v>0.17809093750000002</v>
       </c>
       <c r="B112" s="24">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="C112" s="24">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D112" s="24">
-        <v>7</v>
+        <v>64</v>
       </c>
       <c r="E112" s="24"/>
       <c r="F112" s="24"/>
@@ -3398,16 +3398,16 @@
     </row>
     <row r="113" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="36">
-        <v>0.18865471064814815</v>
+        <v>0.17808966435185186</v>
       </c>
       <c r="B113" s="24">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="C113" s="24">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="D113" s="24">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="E113" s="24"/>
       <c r="F113" s="24"/>
@@ -3419,16 +3419,16 @@
     </row>
     <row r="114" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="36">
-        <v>0.18865350694444444</v>
+        <v>0.17808857638888889</v>
       </c>
       <c r="B114" s="24">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="C114" s="24">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="D114" s="24">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E114" s="24"/>
       <c r="F114" s="24"/>
@@ -3440,16 +3440,16 @@
     </row>
     <row r="115" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="36">
-        <v>0.18865231481481481</v>
+        <v>0.17808731481481482</v>
       </c>
       <c r="B115" s="24">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="C115" s="24">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="D115" s="24">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="E115" s="24"/>
       <c r="F115" s="24"/>
@@ -3460,18 +3460,10 @@
       <c r="K115" s="24"/>
     </row>
     <row r="116" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="36">
-        <v>0.18865122685185184</v>
-      </c>
-      <c r="B116" s="24">
-        <v>45</v>
-      </c>
-      <c r="C116" s="24">
-        <v>32</v>
-      </c>
-      <c r="D116" s="24">
-        <v>7</v>
-      </c>
+      <c r="A116" s="36"/>
+      <c r="B116" s="24"/>
+      <c r="C116" s="24"/>
+      <c r="D116" s="24"/>
       <c r="E116" s="24"/>
       <c r="F116" s="24"/>
       <c r="G116" s="24"/>
@@ -3481,18 +3473,10 @@
       <c r="K116" s="24"/>
     </row>
     <row r="117" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="36">
-        <v>0.18865006944444446</v>
-      </c>
-      <c r="B117" s="24">
-        <v>44</v>
-      </c>
-      <c r="C117" s="24">
-        <v>34</v>
-      </c>
-      <c r="D117" s="24">
-        <v>8</v>
-      </c>
+      <c r="A117" s="36"/>
+      <c r="B117" s="24"/>
+      <c r="C117" s="24"/>
+      <c r="D117" s="24"/>
       <c r="E117" s="24"/>
       <c r="F117" s="24"/>
       <c r="G117" s="24"/>
@@ -3502,18 +3486,10 @@
       <c r="K117" s="24"/>
     </row>
     <row r="118" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="36">
-        <v>0.18864891203703704</v>
-      </c>
-      <c r="B118" s="24">
-        <v>43</v>
-      </c>
-      <c r="C118" s="24">
-        <v>34</v>
-      </c>
-      <c r="D118" s="24">
-        <v>8</v>
-      </c>
+      <c r="A118" s="36"/>
+      <c r="B118" s="24"/>
+      <c r="C118" s="24"/>
+      <c r="D118" s="24"/>
       <c r="E118" s="24"/>
       <c r="F118" s="24"/>
       <c r="G118" s="24"/>
@@ -3523,18 +3499,10 @@
       <c r="K118" s="24"/>
     </row>
     <row r="119" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="36">
-        <v>0.18864770833333333</v>
-      </c>
-      <c r="B119" s="24">
-        <v>41</v>
-      </c>
-      <c r="C119" s="24">
-        <v>33</v>
-      </c>
-      <c r="D119" s="24">
-        <v>6</v>
-      </c>
+      <c r="A119" s="36"/>
+      <c r="B119" s="24"/>
+      <c r="C119" s="24"/>
+      <c r="D119" s="24"/>
       <c r="E119" s="24"/>
       <c r="F119" s="24"/>
       <c r="G119" s="24"/>
@@ -3544,18 +3512,10 @@
       <c r="K119" s="24"/>
     </row>
     <row r="120" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="36">
-        <v>0.18864660879629627</v>
-      </c>
-      <c r="B120" s="24">
-        <v>43</v>
-      </c>
-      <c r="C120" s="24">
-        <v>32</v>
-      </c>
-      <c r="D120" s="24">
-        <v>7</v>
-      </c>
+      <c r="A120" s="36"/>
+      <c r="B120" s="24"/>
+      <c r="C120" s="24"/>
+      <c r="D120" s="24"/>
       <c r="E120" s="24"/>
       <c r="F120" s="24"/>
       <c r="G120" s="24"/>
@@ -3565,18 +3525,10 @@
       <c r="K120" s="24"/>
     </row>
     <row r="121" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="36">
-        <v>0.18864548611111109</v>
-      </c>
-      <c r="B121" s="24">
-        <v>43</v>
-      </c>
-      <c r="C121" s="24">
-        <v>31</v>
-      </c>
-      <c r="D121" s="24">
-        <v>6</v>
-      </c>
+      <c r="A121" s="36"/>
+      <c r="B121" s="24"/>
+      <c r="C121" s="24"/>
+      <c r="D121" s="24"/>
       <c r="E121" s="24"/>
       <c r="F121" s="24"/>
       <c r="G121" s="24"/>
@@ -3586,18 +3538,10 @@
       <c r="K121" s="24"/>
     </row>
     <row r="122" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="36">
-        <v>0.18864430555555556</v>
-      </c>
-      <c r="B122" s="24">
-        <v>41</v>
-      </c>
-      <c r="C122" s="24">
-        <v>30</v>
-      </c>
-      <c r="D122" s="24">
-        <v>6</v>
-      </c>
+      <c r="A122" s="36"/>
+      <c r="B122" s="24"/>
+      <c r="C122" s="24"/>
+      <c r="D122" s="24"/>
       <c r="E122" s="24"/>
       <c r="F122" s="24"/>
       <c r="G122" s="24"/>
@@ -3607,18 +3551,10 @@
       <c r="K122" s="24"/>
     </row>
     <row r="123" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="36">
-        <v>0.18864312499999999</v>
-      </c>
-      <c r="B123" s="24">
-        <v>41</v>
-      </c>
-      <c r="C123" s="24">
-        <v>31</v>
-      </c>
-      <c r="D123" s="24">
-        <v>7</v>
-      </c>
+      <c r="A123" s="36"/>
+      <c r="B123" s="24"/>
+      <c r="C123" s="24"/>
+      <c r="D123" s="24"/>
       <c r="E123" s="24"/>
       <c r="F123" s="24"/>
       <c r="G123" s="24"/>
@@ -3628,18 +3564,10 @@
       <c r="K123" s="24"/>
     </row>
     <row r="124" spans="1:11" ht="16.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="36">
-        <v>0.18864186342592593</v>
-      </c>
-      <c r="B124" s="24">
-        <v>44</v>
-      </c>
-      <c r="C124" s="24">
-        <v>34</v>
-      </c>
-      <c r="D124" s="24">
-        <v>8</v>
-      </c>
+      <c r="A124" s="36"/>
+      <c r="B124" s="24"/>
+      <c r="C124" s="24"/>
+      <c r="D124" s="24"/>
       <c r="E124" s="24"/>
       <c r="F124" s="24"/>
       <c r="G124" s="24"/>

</xml_diff>